<commit_message>
Formed the consolidated report
</commit_message>
<xml_diff>
--- a/tut06/output/2001CB02.xlsx
+++ b/tut06/output/2001CB02.xlsx
@@ -516,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -581,7 +581,9 @@
       <c r="G6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -668,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -689,7 +691,9 @@
       <c r="G11" t="n">
         <v>0</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -732,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -753,7 +757,9 @@
       <c r="G14" t="n">
         <v>0</v>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -862,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -883,7 +889,9 @@
       <c r="G20" t="n">
         <v>0</v>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">

</xml_diff>